<commit_message>
Added comments and improved imports
</commit_message>
<xml_diff>
--- a/input_data/Root Chord Results.xlsx
+++ b/input_data/Root Chord Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rahulrao/Documents/Dev/AeroNU/fin analysis results/input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B143044-E275-1143-9EB1-8ED07DE6D81F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E014A6ED-A887-E642-A38C-88872099AADE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="500" windowWidth="31800" windowHeight="18220" firstSheet="17" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="680" yWindow="500" windowWidth="35160" windowHeight="20660" firstSheet="14" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GG Torque (Z) 20" sheetId="21" r:id="rId1"/>
@@ -10752,7 +10752,7 @@
   <dimension ref="B2:CT25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11055,103 +11055,103 @@
     </row>
     <row r="3" spans="2:98" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="3">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="D3" s="3">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E3" s="3">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="F3" s="3">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="G3" s="3">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="H3" s="3">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="I3" s="3">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="J3" s="3">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="K3" s="3">
-        <v>0.6</v>
+        <v>0.1</v>
       </c>
       <c r="L3" s="3">
-        <v>0.6</v>
+        <v>0.1</v>
       </c>
       <c r="M3" s="3">
-        <v>0.6</v>
+        <v>0.1</v>
       </c>
       <c r="N3" s="3">
-        <v>0.6</v>
+        <v>0.1</v>
       </c>
       <c r="O3" s="3">
-        <v>0.8</v>
+        <v>0.1</v>
       </c>
       <c r="P3" s="3">
-        <v>0.8</v>
+        <v>0.1</v>
       </c>
       <c r="Q3" s="3">
-        <v>0.8</v>
+        <v>0.1</v>
       </c>
       <c r="R3" s="3">
-        <v>0.8</v>
+        <v>0.1</v>
       </c>
       <c r="S3" s="3">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="T3" s="3">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="U3" s="3">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="V3" s="3">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="W3" s="3">
-        <v>0.4</v>
+        <v>0.15</v>
       </c>
       <c r="X3" s="3">
-        <v>0.4</v>
+        <v>0.15</v>
       </c>
       <c r="Y3" s="3">
-        <v>0.4</v>
+        <v>0.15</v>
       </c>
       <c r="Z3" s="3">
-        <v>0.4</v>
+        <v>0.15</v>
       </c>
       <c r="AA3" s="3">
-        <v>0.6</v>
+        <v>0.15</v>
       </c>
       <c r="AB3" s="3">
-        <v>0.6</v>
+        <v>0.15</v>
       </c>
       <c r="AC3" s="3">
-        <v>0.6</v>
+        <v>0.15</v>
       </c>
       <c r="AD3" s="3">
-        <v>0.6</v>
+        <v>0.15</v>
       </c>
       <c r="AE3" s="3">
-        <v>0.8</v>
+        <v>0.15</v>
       </c>
       <c r="AF3" s="3">
-        <v>0.8</v>
+        <v>0.15</v>
       </c>
       <c r="AG3" s="3">
-        <v>0.8</v>
+        <v>0.15</v>
       </c>
       <c r="AH3" s="3">
-        <v>0.8</v>
+        <v>0.15</v>
       </c>
       <c r="AI3" s="3">
         <v>0.2</v>
@@ -11166,770 +11166,770 @@
         <v>0.2</v>
       </c>
       <c r="AM3" s="3">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="AN3" s="3">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="AO3" s="3">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="AP3" s="3">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="AQ3" s="3">
-        <v>0.6</v>
+        <v>0.2</v>
       </c>
       <c r="AR3" s="3">
-        <v>0.6</v>
+        <v>0.2</v>
       </c>
       <c r="AS3" s="3">
-        <v>0.6</v>
+        <v>0.2</v>
       </c>
       <c r="AT3" s="3">
-        <v>0.6</v>
+        <v>0.2</v>
       </c>
       <c r="AU3" s="3">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
       <c r="AV3" s="3">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
       <c r="AW3" s="3">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
       <c r="AX3" s="3">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
       <c r="AY3" s="3">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="AZ3" s="3">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="BA3" s="3">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="BB3" s="3">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="BC3" s="3">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="BD3" s="3">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="BE3" s="3">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="BF3" s="3">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="BG3" s="3">
-        <v>0.6</v>
+        <v>0.25</v>
       </c>
       <c r="BH3" s="3">
-        <v>0.6</v>
+        <v>0.25</v>
       </c>
       <c r="BI3" s="3">
-        <v>0.6</v>
+        <v>0.25</v>
       </c>
       <c r="BJ3" s="3">
-        <v>0.6</v>
+        <v>0.25</v>
       </c>
       <c r="BK3" s="3">
-        <v>0.8</v>
+        <v>0.25</v>
       </c>
       <c r="BL3" s="3">
-        <v>0.8</v>
+        <v>0.25</v>
       </c>
       <c r="BM3" s="3">
-        <v>0.8</v>
+        <v>0.25</v>
       </c>
       <c r="BN3" s="3">
-        <v>0.8</v>
+        <v>0.25</v>
       </c>
       <c r="BO3" s="3">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="BP3" s="3">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="BQ3" s="3">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="BR3" s="3">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="BS3" s="3">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="BT3" s="3">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="BU3" s="3">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="BV3" s="3">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="BW3" s="3">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="BX3" s="3">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="BY3" s="3">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="BZ3" s="3">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="CA3" s="3">
-        <v>0.8</v>
+        <v>0.3</v>
       </c>
       <c r="CB3" s="3">
-        <v>0.8</v>
+        <v>0.3</v>
       </c>
       <c r="CC3" s="3">
-        <v>0.8</v>
+        <v>0.3</v>
       </c>
       <c r="CD3" s="3">
-        <v>0.8</v>
+        <v>0.3</v>
       </c>
       <c r="CE3" s="3">
-        <v>0.2</v>
+        <v>0.35</v>
       </c>
       <c r="CF3" s="3">
-        <v>0.2</v>
+        <v>0.35</v>
       </c>
       <c r="CG3" s="3">
-        <v>0.2</v>
+        <v>0.35</v>
       </c>
       <c r="CH3" s="3">
-        <v>0.2</v>
+        <v>0.35</v>
       </c>
       <c r="CI3" s="3">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
       <c r="CJ3" s="3">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
       <c r="CK3" s="3">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
       <c r="CL3" s="3">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
       <c r="CM3" s="3">
-        <v>0.6</v>
+        <v>0.35</v>
       </c>
       <c r="CN3" s="3">
-        <v>0.6</v>
+        <v>0.35</v>
       </c>
       <c r="CO3" s="3">
-        <v>0.6</v>
+        <v>0.35</v>
       </c>
       <c r="CP3" s="3">
-        <v>0.6</v>
+        <v>0.35</v>
       </c>
       <c r="CQ3" s="3">
-        <v>0.8</v>
+        <v>0.35</v>
       </c>
       <c r="CR3" s="3">
-        <v>0.8</v>
+        <v>0.35</v>
       </c>
       <c r="CS3" s="3">
-        <v>0.8</v>
+        <v>0.35</v>
       </c>
       <c r="CT3" s="3">
-        <v>0.8</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="4" spans="2:98" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="3">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="D4" s="3">
-        <v>2.9088821000000001E-2</v>
+        <v>0.2</v>
       </c>
       <c r="E4" s="3">
-        <v>5.8177642000000002E-2</v>
+        <v>0.2</v>
       </c>
       <c r="F4" s="3">
-        <v>8.7266463000000002E-2</v>
+        <v>0.2</v>
       </c>
       <c r="G4" s="3">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="H4" s="3">
-        <v>2.9088821000000001E-2</v>
+        <v>0.4</v>
       </c>
       <c r="I4" s="3">
-        <v>5.8177642000000002E-2</v>
+        <v>0.4</v>
       </c>
       <c r="J4" s="3">
-        <v>8.7266463000000002E-2</v>
+        <v>0.4</v>
       </c>
       <c r="K4" s="3">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="L4" s="3">
-        <v>2.9088821000000001E-2</v>
+        <v>0.6</v>
       </c>
       <c r="M4" s="3">
-        <v>5.8177642000000002E-2</v>
+        <v>0.6</v>
       </c>
       <c r="N4" s="3">
-        <v>8.7266463000000002E-2</v>
+        <v>0.6</v>
       </c>
       <c r="O4" s="3">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="P4" s="3">
-        <v>2.9088821000000001E-2</v>
+        <v>0.8</v>
       </c>
       <c r="Q4" s="3">
-        <v>5.8177642000000002E-2</v>
+        <v>0.8</v>
       </c>
       <c r="R4" s="3">
-        <v>8.7266463000000002E-2</v>
+        <v>0.8</v>
       </c>
       <c r="S4" s="3">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="T4" s="3">
-        <v>2.9088821000000001E-2</v>
+        <v>0.2</v>
       </c>
       <c r="U4" s="3">
-        <v>5.8177642000000002E-2</v>
+        <v>0.2</v>
       </c>
       <c r="V4" s="3">
-        <v>8.7266463000000002E-2</v>
+        <v>0.2</v>
       </c>
       <c r="W4" s="3">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="X4" s="3">
-        <v>2.9088821000000001E-2</v>
+        <v>0.4</v>
       </c>
       <c r="Y4" s="3">
-        <v>5.8177642000000002E-2</v>
+        <v>0.4</v>
       </c>
       <c r="Z4" s="3">
-        <v>8.7266463000000002E-2</v>
+        <v>0.4</v>
       </c>
       <c r="AA4" s="3">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="AB4" s="3">
-        <v>2.9088821000000001E-2</v>
+        <v>0.6</v>
       </c>
       <c r="AC4" s="3">
-        <v>5.8177642000000002E-2</v>
+        <v>0.6</v>
       </c>
       <c r="AD4" s="3">
-        <v>8.7266463000000002E-2</v>
+        <v>0.6</v>
       </c>
       <c r="AE4" s="3">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="AF4" s="3">
-        <v>2.9088821000000001E-2</v>
+        <v>0.8</v>
       </c>
       <c r="AG4" s="3">
-        <v>5.8177642000000002E-2</v>
+        <v>0.8</v>
       </c>
       <c r="AH4" s="3">
-        <v>8.7266463000000002E-2</v>
+        <v>0.8</v>
       </c>
       <c r="AI4" s="3">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="AJ4" s="3">
-        <v>2.9088821000000001E-2</v>
+        <v>0.2</v>
       </c>
       <c r="AK4" s="3">
-        <v>5.8177642000000002E-2</v>
+        <v>0.2</v>
       </c>
       <c r="AL4" s="3">
-        <v>8.7266463000000002E-2</v>
+        <v>0.2</v>
       </c>
       <c r="AM4" s="3">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="AN4" s="3">
-        <v>2.9088821000000001E-2</v>
+        <v>0.4</v>
       </c>
       <c r="AO4" s="3">
-        <v>5.8177642000000002E-2</v>
+        <v>0.4</v>
       </c>
       <c r="AP4" s="3">
-        <v>8.7266463000000002E-2</v>
+        <v>0.4</v>
       </c>
       <c r="AQ4" s="3">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="AR4" s="3">
-        <v>2.9088821000000001E-2</v>
+        <v>0.6</v>
       </c>
       <c r="AS4" s="3">
-        <v>5.8177642000000002E-2</v>
+        <v>0.6</v>
       </c>
       <c r="AT4" s="3">
-        <v>8.7266463000000002E-2</v>
+        <v>0.6</v>
       </c>
       <c r="AU4" s="3">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="AV4" s="3">
-        <v>2.9088821000000001E-2</v>
+        <v>0.8</v>
       </c>
       <c r="AW4" s="3">
-        <v>5.8177642000000002E-2</v>
+        <v>0.8</v>
       </c>
       <c r="AX4" s="3">
-        <v>8.7266463000000002E-2</v>
+        <v>0.8</v>
       </c>
       <c r="AY4" s="3">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="AZ4" s="3">
-        <v>2.9088821000000001E-2</v>
+        <v>0.2</v>
       </c>
       <c r="BA4" s="3">
-        <v>5.8177642000000002E-2</v>
+        <v>0.2</v>
       </c>
       <c r="BB4" s="3">
-        <v>8.7266463000000002E-2</v>
+        <v>0.2</v>
       </c>
       <c r="BC4" s="3">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="BD4" s="3">
-        <v>2.9088821000000001E-2</v>
+        <v>0.4</v>
       </c>
       <c r="BE4" s="3">
-        <v>5.8177642000000002E-2</v>
+        <v>0.4</v>
       </c>
       <c r="BF4" s="3">
-        <v>8.7266463000000002E-2</v>
+        <v>0.4</v>
       </c>
       <c r="BG4" s="3">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="BH4" s="3">
-        <v>2.9088821000000001E-2</v>
+        <v>0.6</v>
       </c>
       <c r="BI4" s="3">
-        <v>5.8177642000000002E-2</v>
+        <v>0.6</v>
       </c>
       <c r="BJ4" s="3">
-        <v>8.7266463000000002E-2</v>
+        <v>0.6</v>
       </c>
       <c r="BK4" s="3">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="BL4" s="3">
-        <v>2.9088821000000001E-2</v>
+        <v>0.8</v>
       </c>
       <c r="BM4" s="3">
-        <v>5.8177642000000002E-2</v>
+        <v>0.8</v>
       </c>
       <c r="BN4" s="3">
-        <v>8.7266463000000002E-2</v>
+        <v>0.8</v>
       </c>
       <c r="BO4" s="3">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="BP4" s="3">
-        <v>2.9088821000000001E-2</v>
+        <v>0.2</v>
       </c>
       <c r="BQ4" s="3">
-        <v>5.8177642000000002E-2</v>
+        <v>0.2</v>
       </c>
       <c r="BR4" s="3">
-        <v>8.7266463000000002E-2</v>
+        <v>0.2</v>
       </c>
       <c r="BS4" s="3">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="BT4" s="3">
-        <v>2.9088821000000001E-2</v>
+        <v>0.4</v>
       </c>
       <c r="BU4" s="3">
-        <v>5.8177642000000002E-2</v>
+        <v>0.4</v>
       </c>
       <c r="BV4" s="3">
-        <v>8.7266463000000002E-2</v>
+        <v>0.4</v>
       </c>
       <c r="BW4" s="3">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="BX4" s="3">
-        <v>2.9088821000000001E-2</v>
+        <v>0.6</v>
       </c>
       <c r="BY4" s="3">
-        <v>5.8177642000000002E-2</v>
+        <v>0.6</v>
       </c>
       <c r="BZ4" s="3">
-        <v>8.7266463000000002E-2</v>
+        <v>0.6</v>
       </c>
       <c r="CA4" s="3">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="CB4" s="3">
-        <v>2.9088821000000001E-2</v>
+        <v>0.8</v>
       </c>
       <c r="CC4" s="3">
-        <v>5.8177642000000002E-2</v>
+        <v>0.8</v>
       </c>
       <c r="CD4" s="3">
-        <v>8.7266463000000002E-2</v>
+        <v>0.8</v>
       </c>
       <c r="CE4" s="3">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="CF4" s="3">
-        <v>2.9088821000000001E-2</v>
+        <v>0.2</v>
       </c>
       <c r="CG4" s="3">
-        <v>5.8177642000000002E-2</v>
+        <v>0.2</v>
       </c>
       <c r="CH4" s="3">
-        <v>8.7266463000000002E-2</v>
+        <v>0.2</v>
       </c>
       <c r="CI4" s="3">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="CJ4" s="3">
-        <v>2.9088821000000001E-2</v>
+        <v>0.4</v>
       </c>
       <c r="CK4" s="3">
-        <v>5.8177642000000002E-2</v>
+        <v>0.4</v>
       </c>
       <c r="CL4" s="3">
-        <v>8.7266463000000002E-2</v>
+        <v>0.4</v>
       </c>
       <c r="CM4" s="3">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="CN4" s="3">
-        <v>2.9088821000000001E-2</v>
+        <v>0.6</v>
       </c>
       <c r="CO4" s="3">
-        <v>5.8177642000000002E-2</v>
+        <v>0.6</v>
       </c>
       <c r="CP4" s="3">
-        <v>8.7266463000000002E-2</v>
+        <v>0.6</v>
       </c>
       <c r="CQ4" s="3">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="CR4" s="3">
-        <v>2.9088821000000001E-2</v>
+        <v>0.8</v>
       </c>
       <c r="CS4" s="3">
-        <v>5.8177642000000002E-2</v>
+        <v>0.8</v>
       </c>
       <c r="CT4" s="3">
-        <v>8.7266463000000002E-2</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="5" spans="2:98" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="3">
         <v>0</v>
       </c>
-      <c r="C5" s="3">
-        <v>0.1</v>
-      </c>
       <c r="D5" s="3">
-        <v>0.1</v>
+        <v>2.9088821000000001E-2</v>
       </c>
       <c r="E5" s="3">
-        <v>0.1</v>
+        <v>5.8177642000000002E-2</v>
       </c>
       <c r="F5" s="3">
-        <v>0.1</v>
+        <v>8.7266463000000002E-2</v>
       </c>
       <c r="G5" s="3">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="H5" s="3">
-        <v>0.1</v>
+        <v>2.9088821000000001E-2</v>
       </c>
       <c r="I5" s="3">
-        <v>0.1</v>
+        <v>5.8177642000000002E-2</v>
       </c>
       <c r="J5" s="3">
-        <v>0.1</v>
+        <v>8.7266463000000002E-2</v>
       </c>
       <c r="K5" s="3">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="L5" s="3">
-        <v>0.1</v>
+        <v>2.9088821000000001E-2</v>
       </c>
       <c r="M5" s="3">
-        <v>0.1</v>
+        <v>5.8177642000000002E-2</v>
       </c>
       <c r="N5" s="3">
-        <v>0.1</v>
+        <v>8.7266463000000002E-2</v>
       </c>
       <c r="O5" s="3">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="P5" s="3">
-        <v>0.1</v>
+        <v>2.9088821000000001E-2</v>
       </c>
       <c r="Q5" s="3">
-        <v>0.1</v>
+        <v>5.8177642000000002E-2</v>
       </c>
       <c r="R5" s="3">
-        <v>0.1</v>
+        <v>8.7266463000000002E-2</v>
       </c>
       <c r="S5" s="3">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="T5" s="3">
-        <v>0.15</v>
+        <v>2.9088821000000001E-2</v>
       </c>
       <c r="U5" s="3">
-        <v>0.15</v>
+        <v>5.8177642000000002E-2</v>
       </c>
       <c r="V5" s="3">
-        <v>0.15</v>
+        <v>8.7266463000000002E-2</v>
       </c>
       <c r="W5" s="3">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="X5" s="3">
-        <v>0.15</v>
+        <v>2.9088821000000001E-2</v>
       </c>
       <c r="Y5" s="3">
-        <v>0.15</v>
+        <v>5.8177642000000002E-2</v>
       </c>
       <c r="Z5" s="3">
-        <v>0.15</v>
+        <v>8.7266463000000002E-2</v>
       </c>
       <c r="AA5" s="3">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="AB5" s="3">
-        <v>0.15</v>
+        <v>2.9088821000000001E-2</v>
       </c>
       <c r="AC5" s="3">
-        <v>0.15</v>
+        <v>5.8177642000000002E-2</v>
       </c>
       <c r="AD5" s="3">
-        <v>0.15</v>
+        <v>8.7266463000000002E-2</v>
       </c>
       <c r="AE5" s="3">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="AF5" s="3">
-        <v>0.15</v>
+        <v>2.9088821000000001E-2</v>
       </c>
       <c r="AG5" s="3">
-        <v>0.15</v>
+        <v>5.8177642000000002E-2</v>
       </c>
       <c r="AH5" s="3">
-        <v>0.15</v>
+        <v>8.7266463000000002E-2</v>
       </c>
       <c r="AI5" s="3">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="AJ5" s="3">
-        <v>0.2</v>
+        <v>2.9088821000000001E-2</v>
       </c>
       <c r="AK5" s="3">
-        <v>0.2</v>
+        <v>5.8177642000000002E-2</v>
       </c>
       <c r="AL5" s="3">
-        <v>0.2</v>
+        <v>8.7266463000000002E-2</v>
       </c>
       <c r="AM5" s="3">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="AN5" s="3">
-        <v>0.2</v>
+        <v>2.9088821000000001E-2</v>
       </c>
       <c r="AO5" s="3">
-        <v>0.2</v>
+        <v>5.8177642000000002E-2</v>
       </c>
       <c r="AP5" s="3">
-        <v>0.2</v>
+        <v>8.7266463000000002E-2</v>
       </c>
       <c r="AQ5" s="3">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="AR5" s="3">
-        <v>0.2</v>
+        <v>2.9088821000000001E-2</v>
       </c>
       <c r="AS5" s="3">
-        <v>0.2</v>
+        <v>5.8177642000000002E-2</v>
       </c>
       <c r="AT5" s="3">
-        <v>0.2</v>
+        <v>8.7266463000000002E-2</v>
       </c>
       <c r="AU5" s="3">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="AV5" s="3">
-        <v>0.2</v>
+        <v>2.9088821000000001E-2</v>
       </c>
       <c r="AW5" s="3">
-        <v>0.2</v>
+        <v>5.8177642000000002E-2</v>
       </c>
       <c r="AX5" s="3">
-        <v>0.2</v>
+        <v>8.7266463000000002E-2</v>
       </c>
       <c r="AY5" s="3">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="AZ5" s="3">
-        <v>0.25</v>
+        <v>2.9088821000000001E-2</v>
       </c>
       <c r="BA5" s="3">
-        <v>0.25</v>
+        <v>5.8177642000000002E-2</v>
       </c>
       <c r="BB5" s="3">
-        <v>0.25</v>
+        <v>8.7266463000000002E-2</v>
       </c>
       <c r="BC5" s="3">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="BD5" s="3">
-        <v>0.25</v>
+        <v>2.9088821000000001E-2</v>
       </c>
       <c r="BE5" s="3">
-        <v>0.25</v>
+        <v>5.8177642000000002E-2</v>
       </c>
       <c r="BF5" s="3">
-        <v>0.25</v>
+        <v>8.7266463000000002E-2</v>
       </c>
       <c r="BG5" s="3">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="BH5" s="3">
-        <v>0.25</v>
+        <v>2.9088821000000001E-2</v>
       </c>
       <c r="BI5" s="3">
-        <v>0.25</v>
+        <v>5.8177642000000002E-2</v>
       </c>
       <c r="BJ5" s="3">
-        <v>0.25</v>
+        <v>8.7266463000000002E-2</v>
       </c>
       <c r="BK5" s="3">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="BL5" s="3">
-        <v>0.25</v>
+        <v>2.9088821000000001E-2</v>
       </c>
       <c r="BM5" s="3">
-        <v>0.25</v>
+        <v>5.8177642000000002E-2</v>
       </c>
       <c r="BN5" s="3">
-        <v>0.25</v>
+        <v>8.7266463000000002E-2</v>
       </c>
       <c r="BO5" s="3">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="BP5" s="3">
-        <v>0.3</v>
+        <v>2.9088821000000001E-2</v>
       </c>
       <c r="BQ5" s="3">
-        <v>0.3</v>
+        <v>5.8177642000000002E-2</v>
       </c>
       <c r="BR5" s="3">
-        <v>0.3</v>
+        <v>8.7266463000000002E-2</v>
       </c>
       <c r="BS5" s="3">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="BT5" s="3">
-        <v>0.3</v>
+        <v>2.9088821000000001E-2</v>
       </c>
       <c r="BU5" s="3">
-        <v>0.3</v>
+        <v>5.8177642000000002E-2</v>
       </c>
       <c r="BV5" s="3">
-        <v>0.3</v>
+        <v>8.7266463000000002E-2</v>
       </c>
       <c r="BW5" s="3">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="BX5" s="3">
-        <v>0.3</v>
+        <v>2.9088821000000001E-2</v>
       </c>
       <c r="BY5" s="3">
-        <v>0.3</v>
+        <v>5.8177642000000002E-2</v>
       </c>
       <c r="BZ5" s="3">
-        <v>0.3</v>
+        <v>8.7266463000000002E-2</v>
       </c>
       <c r="CA5" s="3">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="CB5" s="3">
-        <v>0.3</v>
+        <v>2.9088821000000001E-2</v>
       </c>
       <c r="CC5" s="3">
-        <v>0.3</v>
+        <v>5.8177642000000002E-2</v>
       </c>
       <c r="CD5" s="3">
-        <v>0.3</v>
+        <v>8.7266463000000002E-2</v>
       </c>
       <c r="CE5" s="3">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="CF5" s="3">
-        <v>0.35</v>
+        <v>2.9088821000000001E-2</v>
       </c>
       <c r="CG5" s="3">
-        <v>0.35</v>
+        <v>5.8177642000000002E-2</v>
       </c>
       <c r="CH5" s="3">
-        <v>0.35</v>
+        <v>8.7266463000000002E-2</v>
       </c>
       <c r="CI5" s="3">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="CJ5" s="3">
-        <v>0.35</v>
+        <v>2.9088821000000001E-2</v>
       </c>
       <c r="CK5" s="3">
-        <v>0.35</v>
+        <v>5.8177642000000002E-2</v>
       </c>
       <c r="CL5" s="3">
-        <v>0.35</v>
+        <v>8.7266463000000002E-2</v>
       </c>
       <c r="CM5" s="3">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="CN5" s="3">
-        <v>0.35</v>
+        <v>2.9088821000000001E-2</v>
       </c>
       <c r="CO5" s="3">
-        <v>0.35</v>
+        <v>5.8177642000000002E-2</v>
       </c>
       <c r="CP5" s="3">
-        <v>0.35</v>
+        <v>8.7266463000000002E-2</v>
       </c>
       <c r="CQ5" s="3">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="CR5" s="3">
-        <v>0.35</v>
+        <v>2.9088821000000001E-2</v>
       </c>
       <c r="CS5" s="3">
-        <v>0.35</v>
+        <v>5.8177642000000002E-2</v>
       </c>
       <c r="CT5" s="3">
-        <v>0.35</v>
+        <v>8.7266463000000002E-2</v>
       </c>
     </row>
     <row r="6" spans="2:98" x14ac:dyDescent="0.2">

</xml_diff>